<commit_message>
Update Tabela Dicionario de Dados
Correção no erro da tabela de dicionario de dados
</commit_message>
<xml_diff>
--- a/Modelagem/Dicionario de Dados.xlsx
+++ b/Modelagem/Dicionario de Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamily.luzes\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178C80DE-736B-4415-99B5-9B44CB38CADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741113A3-EB92-4C94-A452-45157E11AF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="11" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
     <sheet name="Fornecedores" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -145,9 +144,6 @@
     <t>1 - sem limite</t>
   </si>
   <si>
-    <t>Varchar(18)</t>
-  </si>
-  <si>
     <t>10-15</t>
   </si>
   <si>
@@ -878,6 +874,9 @@
   </si>
   <si>
     <t>Tabela responsável por armazenar os dados das empresas ou pessoas jurídicas que fornecem serviços ou equipamentos.</t>
+  </si>
+  <si>
+    <t>Varchar(11)</t>
   </si>
 </sst>
 </file>
@@ -1034,6 +1033,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1042,9 +1044,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1377,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1392,47 +1391,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1453,10 +1452,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1471,19 +1470,19 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -1491,16 +1490,16 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>277</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>29</v>
@@ -1511,14 +1510,14 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
@@ -1531,19 +1530,19 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>9</v>
@@ -1551,14 +1550,14 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="16"/>
+      <c r="A10" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1573,27 +1572,27 @@
         <v>20</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1603,17 +1602,17 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="A13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1621,17 +1620,17 @@
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3" t="s">
         <v>10</v>
@@ -1639,17 +1638,17 @@
       <c r="E14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="F14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="18"/>
+      <c r="A15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3" t="s">
         <v>10</v>
@@ -1657,56 +1656,46 @@
       <c r="E15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="F15" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="A16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="15"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="F16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="18"/>
+      <c r="A17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="F17" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:H15"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="B1:H1"/>
@@ -1720,6 +1709,16 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:H15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1752,47 +1751,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1813,10 +1812,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1831,14 +1830,14 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
         <v>21</v>
       </c>
@@ -1853,14 +1852,14 @@
         <v>20</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="17"/>
       <c r="C7" s="14" t="s">
         <v>21</v>
       </c>
@@ -1875,19 +1874,19 @@
         <v>20</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="B8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>9</v>
@@ -1895,39 +1894,39 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>222</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="14" t="s">
-        <v>224</v>
-      </c>
       <c r="D10" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>9</v>
@@ -1935,19 +1934,19 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="14" t="s">
-        <v>109</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>9</v>
@@ -1955,26 +1954,26 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
@@ -1984,17 +1983,17 @@
       <c r="E13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A14" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
@@ -2002,62 +2001,76 @@
       <c r="E14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="F14" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="B15" s="18"/>
+      <c r="A15" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="4"/>
       <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4"/>
       <c r="D16" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="4"/>
       <c r="D17" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="12"/>
-      <c r="F17" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="F17" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="A14:B14"/>
@@ -2066,20 +2079,6 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2108,47 +2107,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
@@ -2169,10 +2168,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
         <v>21</v>
       </c>
@@ -2187,14 +2186,14 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
         <v>21</v>
       </c>
@@ -2209,19 +2208,19 @@
         <v>20</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="17"/>
       <c r="C7" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>9</v>
@@ -2229,19 +2228,19 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="14" t="s">
-        <v>109</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>9</v>
@@ -2249,19 +2248,19 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="B9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" s="17"/>
       <c r="C9" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>9</v>
@@ -2269,19 +2268,19 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>245</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>9</v>
@@ -2289,26 +2288,26 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
@@ -2318,17 +2317,17 @@
       <c r="E12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="A13" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
@@ -2336,62 +2335,73 @@
       <c r="E13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="F13" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A14" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="4"/>
       <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="4"/>
       <c r="D15" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4"/>
       <c r="D16" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="F16" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="A16:B16"/>
@@ -2402,17 +2412,6 @@
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2422,7 +2421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A55FCD8-AAC8-4D8D-A092-A88F3F334D41}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
@@ -2441,47 +2440,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
@@ -2502,10 +2501,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
         <v>21</v>
       </c>
@@ -2520,14 +2519,14 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
@@ -2540,19 +2539,19 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>265</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>266</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>9</v>
@@ -2560,19 +2559,19 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="B8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>9</v>
@@ -2580,26 +2579,26 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="13" t="s">
         <v>11</v>
       </c>
@@ -2609,17 +2608,17 @@
       <c r="E10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="B11" s="18"/>
+      <c r="A11" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2627,17 +2626,17 @@
       <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="F11" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="B12" s="18"/>
+      <c r="A12" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="4"/>
       <c r="D12" s="12" t="s">
         <v>10</v>
@@ -2645,47 +2644,47 @@
       <c r="E12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="4"/>
       <c r="D13" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="F13" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2714,47 +2713,47 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
@@ -2775,10 +2774,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
@@ -2793,14 +2792,14 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
@@ -2813,19 +2812,19 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>9</v>
@@ -2833,19 +2832,19 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
@@ -2853,26 +2852,26 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="8" t="s">
         <v>11</v>
       </c>
@@ -2882,17 +2881,17 @@
       <c r="E10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="18"/>
+      <c r="A11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2900,33 +2899,33 @@
       <c r="E11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="F11" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="18"/>
+      <c r="A12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="4"/>
       <c r="D12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="4"/>
       <c r="D13" s="10" t="s">
         <v>10</v>
@@ -2934,31 +2933,31 @@
       <c r="E13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="F13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
@@ -2990,47 +2989,47 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
@@ -3051,10 +3050,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
@@ -3069,19 +3068,19 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>9</v>
@@ -3089,19 +3088,19 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>9</v>
@@ -3109,19 +3108,19 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
@@ -3129,39 +3128,39 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="17"/>
       <c r="C9" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="16"/>
+      <c r="A10" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>9</v>
@@ -3169,19 +3168,19 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>9</v>
@@ -3189,19 +3188,19 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>9</v>
@@ -3209,26 +3208,26 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
@@ -3238,17 +3237,17 @@
       <c r="E14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="18"/>
+      <c r="A15" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
@@ -3256,52 +3255,46 @@
       <c r="E15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4"/>
       <c r="D16" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="F16" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="18"/>
+      <c r="A17" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="4"/>
       <c r="D17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="F17" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="A7:B7"/>
@@ -3317,6 +3310,12 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
@@ -3349,47 +3348,47 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
@@ -3410,10 +3409,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
@@ -3428,19 +3427,19 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>107</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>9</v>
@@ -3448,19 +3447,19 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>9</v>
@@ -3468,26 +3467,26 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
@@ -3497,17 +3496,17 @@
       <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="18"/>
+      <c r="A10" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="15"/>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
@@ -3515,17 +3514,17 @@
       <c r="E10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="F10" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="18"/>
+      <c r="A11" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="4"/>
       <c r="D11" s="10" t="s">
         <v>10</v>
@@ -3533,20 +3532,14 @@
       <c r="E11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="F11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="A11:B11"/>
@@ -3555,6 +3548,12 @@
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
@@ -3586,47 +3585,47 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
@@ -3647,10 +3646,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
@@ -3665,14 +3664,14 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
@@ -3685,14 +3684,14 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="9" t="s">
         <v>26</v>
       </c>
@@ -3705,19 +3704,19 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
@@ -3725,19 +3724,19 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="9" t="s">
-        <v>125</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>9</v>
@@ -3745,19 +3744,19 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>9</v>
@@ -3765,19 +3764,19 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>9</v>
@@ -3787,7 +3786,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -3803,10 +3802,10 @@
       <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="8" t="s">
         <v>11</v>
       </c>
@@ -3816,17 +3815,17 @@
       <c r="E13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A14" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
@@ -3834,17 +3833,17 @@
       <c r="E14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="F14" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" s="18"/>
+      <c r="A15" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="4"/>
       <c r="D15" s="10" t="s">
         <v>10</v>
@@ -3852,73 +3851,62 @@
       <c r="E15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="F15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="A16" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="15"/>
       <c r="C16" s="4"/>
       <c r="D16" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="F16" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="18"/>
+      <c r="A17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="4"/>
       <c r="D17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="F17" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" s="18"/>
+      <c r="A18" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="15"/>
       <c r="C18" s="4"/>
       <c r="D18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+      <c r="F18" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:H12"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="A18:B18"/>
@@ -3932,6 +3920,17 @@
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
@@ -3963,47 +3962,47 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
@@ -4024,10 +4023,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
@@ -4042,14 +4041,14 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="17"/>
       <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
@@ -4064,19 +4063,19 @@
         <v>20</v>
       </c>
       <c r="H6" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>9</v>
@@ -4084,19 +4083,19 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
@@ -4104,19 +4103,19 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>9</v>
@@ -4124,26 +4123,26 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
@@ -4153,17 +4152,17 @@
       <c r="E11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="18"/>
+      <c r="A12" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
@@ -4171,62 +4170,70 @@
       <c r="E12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="F12" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="A13" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="4"/>
       <c r="D13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="4"/>
       <c r="D14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="4"/>
       <c r="D15" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="F15" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="B1:H1"/>
@@ -4239,14 +4246,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4275,47 +4274,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
@@ -4336,10 +4335,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4354,14 +4353,14 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
         <v>21</v>
       </c>
@@ -4376,14 +4375,14 @@
         <v>20</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="17"/>
       <c r="C7" s="14" t="s">
         <v>21</v>
       </c>
@@ -4398,19 +4397,19 @@
         <v>20</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>9</v>
@@ -4418,39 +4417,39 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="17"/>
       <c r="C9" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="14" t="s">
-        <v>173</v>
-      </c>
       <c r="D10" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>9</v>
@@ -4458,26 +4457,26 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
@@ -4487,17 +4486,17 @@
       <c r="E12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="A13" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
@@ -4505,62 +4504,75 @@
       <c r="E13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="F13" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A14" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="4"/>
       <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="4"/>
       <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4"/>
       <c r="D16" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="F16" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="A13:B13"/>
@@ -4569,19 +4581,6 @@
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4608,47 +4607,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
@@ -4669,10 +4668,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4689,14 +4688,14 @@
         <v>20</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
         <v>21</v>
       </c>
@@ -4713,19 +4712,19 @@
         <v>20</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="17"/>
       <c r="C7" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>9</v>
@@ -4733,19 +4732,19 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>9</v>
@@ -4753,26 +4752,26 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="13" t="s">
         <v>11</v>
       </c>
@@ -4782,17 +4781,17 @@
       <c r="E10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="B11" s="18"/>
+      <c r="A11" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -4800,30 +4799,36 @@
       <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4"/>
       <c r="D12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="F12" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A12:B12"/>
@@ -4833,12 +4838,6 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4867,47 +4866,47 @@
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
@@ -4928,10 +4927,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4946,14 +4945,14 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
         <v>21</v>
       </c>
@@ -4968,19 +4967,19 @@
         <v>20</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="17"/>
       <c r="C7" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>9</v>
@@ -4988,19 +4987,19 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>9</v>
@@ -5008,19 +5007,19 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="17"/>
       <c r="C9" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>9</v>
@@ -5028,26 +5027,26 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="13" t="s">
         <v>11</v>
       </c>
@@ -5057,17 +5056,17 @@
       <c r="E11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="B12" s="18"/>
+      <c r="A12" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
@@ -5075,64 +5074,64 @@
       <c r="E12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="F12" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="B13" s="18"/>
+      <c r="A13" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="4"/>
       <c r="D13" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="4"/>
       <c r="D14" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="F14" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>